<commit_message>
email logs html, drop feature added
</commit_message>
<xml_diff>
--- a/public/mm_template.xlsx
+++ b/public/mm_template.xlsx
@@ -20,18 +20,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve">OA</t>
   </si>
   <si>
-    <t xml:space="preserve">MM#</t>
+    <t xml:space="preserve">MMNo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MMDescription</t>
   </si>
   <si>
     <t xml:space="preserve">Qty</t>
   </si>
   <si>
-    <t xml:space="preserve">Plant Code</t>
+    <t xml:space="preserve">UnitPrice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PlantCode</t>
   </si>
 </sst>
 </file>
@@ -114,7 +120,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -125,6 +131,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -320,40 +330,46 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.515625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="37.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="12.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="37.27"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E2" s="1"/>
-      <c r="F2" s="3"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>